<commit_message>
updateTestStands and updated firmware source
Updated optics_module_testStand_***** for testing optics
Updated source code for the controlBoard, interfaceBoard and
imagingBoard
They now contain all combinations of exports from the online compiler
</commit_message>
<xml_diff>
--- a/info/licenseInfo/DIY 3D Printable Raspberry Pi Raman Spectrometer License and Library Information.xlsx
+++ b/info/licenseInfo/DIY 3D Printable Raspberry Pi Raman Spectrometer License and Library Information.xlsx
@@ -212,6 +212,54 @@
   </si>
   <si>
     <t>http://mbed.org/users/simonbarker/code/HIH-4030/</t>
+  </si>
+  <si>
+    <t>Contributor Agreement</t>
+  </si>
+  <si>
+    <t>https://mbed.org/contributor_agreement/</t>
+  </si>
+  <si>
+    <t>TFT_ILI9341 Color Display</t>
+  </si>
+  <si>
+    <t>http://www.eBay.com</t>
+  </si>
+  <si>
+    <t>TFT LCD</t>
+  </si>
+  <si>
+    <t>N/A ?</t>
+  </si>
+  <si>
+    <t>Peter Drescher / library for SPI_TFT_ILI9341</t>
+  </si>
+  <si>
+    <t>http://mbed.org/users/dreschpe/code/SPI_TFT_ILI9341/</t>
+  </si>
+  <si>
+    <t>Contributor Agreement</t>
+  </si>
+  <si>
+    <t>https://mbed.org/contributor_agreement/</t>
+  </si>
+  <si>
+    <t>DS18B20 Temperature Sensor</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/381</t>
+  </si>
+  <si>
+    <t>PID: 381</t>
+  </si>
+  <si>
+    <t>N/A ?</t>
+  </si>
+  <si>
+    <t>Tony Mudd / library for MultipleDS18B20</t>
+  </si>
+  <si>
+    <t>http://mbed.org/users/tonymudd/code/MultipleDS18B20/</t>
   </si>
   <si>
     <t>Contributor Agreement</t>
@@ -1228,144 +1276,144 @@
       </c>
     </row>
     <row r="11">
-      <c t="s" s="22" r="A11">
+      <c t="s" s="1" r="A11">
         <v>69</v>
       </c>
-      <c s="23" r="B11"/>
-      <c s="23" r="C11"/>
-      <c s="23" r="D11"/>
-      <c s="24" r="E11"/>
-      <c s="23" r="F11"/>
-      <c s="23" r="G11"/>
-      <c s="23" r="H11"/>
-      <c s="23" r="I11"/>
-      <c s="23" r="J11"/>
-      <c s="23" r="K11"/>
-      <c s="23" r="L11"/>
-      <c s="23" r="M11"/>
-      <c s="23" r="N11"/>
-      <c s="23" r="O11"/>
-      <c s="23" r="P11"/>
-      <c s="23" r="Q11"/>
-      <c s="23" r="R11"/>
-      <c s="23" r="S11"/>
-      <c s="23" r="T11"/>
-      <c s="23" r="U11"/>
-      <c s="23" r="V11"/>
-      <c s="23" r="W11"/>
-      <c s="23" r="X11"/>
-      <c s="23" r="Y11"/>
-      <c s="25" r="Z11"/>
+      <c t="s" s="15" r="B11">
+        <v>70</v>
+      </c>
+      <c t="s" s="21" r="C11">
+        <v>71</v>
+      </c>
+      <c t="s" s="11" r="D11">
+        <v>72</v>
+      </c>
+      <c s="18" r="E11"/>
+      <c t="s" s="13" r="F11">
+        <v>73</v>
+      </c>
+      <c t="s" s="17" r="G11">
+        <v>74</v>
+      </c>
+      <c t="s" s="11" r="H11">
+        <v>75</v>
+      </c>
+      <c t="s" s="16" r="I11">
+        <v>76</v>
+      </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>70</v>
-      </c>
-      <c t="str" s="10" r="B12">
+        <v>77</v>
+      </c>
+      <c t="s" s="15" r="B12">
+        <v>78</v>
+      </c>
+      <c t="s" s="21" r="C12">
+        <v>79</v>
+      </c>
+      <c t="s" s="11" r="D12">
+        <v>80</v>
+      </c>
+      <c s="18" r="E12"/>
+      <c t="s" s="13" r="F12">
+        <v>81</v>
+      </c>
+      <c t="s" s="17" r="G12">
+        <v>82</v>
+      </c>
+      <c t="s" s="11" r="H12">
+        <v>83</v>
+      </c>
+      <c t="s" s="16" r="I12">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="22" r="A13">
+        <v>85</v>
+      </c>
+      <c s="23" r="B13"/>
+      <c s="23" r="C13"/>
+      <c s="23" r="D13"/>
+      <c s="24" r="E13"/>
+      <c s="23" r="F13"/>
+      <c s="23" r="G13"/>
+      <c s="23" r="H13"/>
+      <c s="23" r="I13"/>
+      <c s="23" r="J13"/>
+      <c s="23" r="K13"/>
+      <c s="23" r="L13"/>
+      <c s="23" r="M13"/>
+      <c s="23" r="N13"/>
+      <c s="23" r="O13"/>
+      <c s="23" r="P13"/>
+      <c s="23" r="Q13"/>
+      <c s="23" r="R13"/>
+      <c s="23" r="S13"/>
+      <c s="23" r="T13"/>
+      <c s="23" r="U13"/>
+      <c s="23" r="V13"/>
+      <c s="23" r="W13"/>
+      <c s="23" r="X13"/>
+      <c s="23" r="Y13"/>
+      <c s="25" r="Z13"/>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>86</v>
+      </c>
+      <c t="str" s="10" r="B14">
         <f>HYPERLINK("http://www.digilentinc.com/Products/Detail.cfm?Prod=CHIPKIT-UNO32","chipKit Uno32")</f>
         <v>chipKit Uno32</v>
       </c>
-      <c t="s" s="1" r="C12">
-        <v>71</v>
-      </c>
-      <c t="s" s="11" r="D12">
-        <v>72</v>
-      </c>
-      <c t="s" s="16" r="E12">
-        <v>73</v>
-      </c>
-      <c t="s" s="13" r="F12">
-        <v>74</v>
-      </c>
-      <c t="s" s="17" r="G12">
-        <v>75</v>
-      </c>
-      <c s="3" r="H12"/>
-      <c s="3" r="I12"/>
-    </row>
-    <row r="13">
-      <c t="s" s="26" r="A13">
-        <v>76</v>
-      </c>
-      <c s="27" r="B13"/>
-      <c s="27" r="C13"/>
-      <c s="27" r="D13"/>
-      <c s="27" r="E13"/>
-      <c s="27" r="F13"/>
-      <c s="27" r="G13"/>
-      <c s="27" r="H13"/>
-      <c s="27" r="I13"/>
-      <c s="27" r="J13"/>
-      <c s="27" r="K13"/>
-      <c s="27" r="L13"/>
-      <c s="27" r="M13"/>
-      <c s="27" r="N13"/>
-      <c s="27" r="O13"/>
-      <c s="27" r="P13"/>
-      <c s="27" r="Q13"/>
-      <c s="27" r="R13"/>
-      <c s="27" r="S13"/>
-      <c s="27" r="T13"/>
-      <c s="27" r="U13"/>
-      <c s="27" r="V13"/>
-      <c s="27" r="W13"/>
-      <c s="27" r="X13"/>
-      <c s="27" r="Y13"/>
-      <c s="28" r="Z13"/>
-    </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
-        <v>77</v>
-      </c>
-      <c t="s" s="15" r="B14">
-        <v>78</v>
-      </c>
       <c t="s" s="1" r="C14">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c t="s" s="11" r="D14">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c t="s" s="16" r="E14">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c t="s" s="13" r="F14">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c t="s" s="17" r="G14">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c s="3" r="H14"/>
       <c s="3" r="I14"/>
     </row>
     <row r="15">
-      <c t="s" s="1" r="A15">
-        <v>84</v>
-      </c>
-      <c t="s" s="15" r="B15">
-        <v>85</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>86</v>
-      </c>
-      <c t="s" s="19" r="D15">
-        <v>87</v>
-      </c>
-      <c t="s" s="18" r="E15">
-        <v>88</v>
-      </c>
-      <c t="s" s="13" r="F15">
-        <v>89</v>
-      </c>
-      <c t="s" s="17" r="G15">
-        <v>90</v>
-      </c>
-      <c t="s" s="11" r="H15">
-        <v>91</v>
-      </c>
-      <c t="s" s="16" r="I15">
+      <c t="s" s="26" r="A15">
         <v>92</v>
       </c>
+      <c s="27" r="B15"/>
+      <c s="27" r="C15"/>
+      <c s="27" r="D15"/>
+      <c s="27" r="E15"/>
+      <c s="27" r="F15"/>
+      <c s="27" r="G15"/>
+      <c s="27" r="H15"/>
+      <c s="27" r="I15"/>
+      <c s="27" r="J15"/>
+      <c s="27" r="K15"/>
+      <c s="27" r="L15"/>
+      <c s="27" r="M15"/>
+      <c s="27" r="N15"/>
+      <c s="27" r="O15"/>
+      <c s="27" r="P15"/>
+      <c s="27" r="Q15"/>
+      <c s="27" r="R15"/>
+      <c s="27" r="S15"/>
+      <c s="27" r="T15"/>
+      <c s="27" r="U15"/>
+      <c s="27" r="V15"/>
+      <c s="27" r="W15"/>
+      <c s="27" r="X15"/>
+      <c s="27" r="Y15"/>
+      <c s="28" r="Z15"/>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
@@ -1377,167 +1425,166 @@
       <c t="s" s="1" r="C16">
         <v>95</v>
       </c>
-      <c t="s" s="19" r="D16">
+      <c t="s" s="11" r="D16">
         <v>96</v>
       </c>
-      <c t="s" s="18" r="E16">
+      <c t="s" s="16" r="E16">
         <v>97</v>
       </c>
       <c t="s" s="13" r="F16">
         <v>98</v>
       </c>
-      <c t="s" s="20" r="G16">
+      <c t="s" s="17" r="G16">
         <v>99</v>
       </c>
-      <c t="s" s="11" r="H16">
+      <c s="3" r="H16"/>
+      <c s="3" r="I16"/>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
         <v>100</v>
       </c>
-      <c t="s" s="16" r="I16">
+      <c t="s" s="15" r="B17">
         <v>101</v>
       </c>
-    </row>
-    <row r="17">
-      <c t="s" s="29" r="A17">
+      <c t="s" s="1" r="C17">
         <v>102</v>
       </c>
-      <c s="30" r="B17"/>
-      <c s="30" r="C17"/>
-      <c s="30" r="D17"/>
-      <c s="30" r="E17"/>
-      <c s="30" r="F17"/>
-      <c s="30" r="G17"/>
-      <c s="30" r="H17"/>
-      <c s="30" r="I17"/>
-      <c s="30" r="J17"/>
-      <c s="30" r="K17"/>
-      <c s="30" r="L17"/>
-      <c s="30" r="M17"/>
-      <c s="30" r="N17"/>
-      <c s="30" r="O17"/>
-      <c s="30" r="P17"/>
-      <c s="30" r="Q17"/>
-      <c s="30" r="R17"/>
-      <c s="30" r="S17"/>
-      <c s="30" r="T17"/>
-      <c s="30" r="U17"/>
-      <c s="30" r="V17"/>
-      <c s="30" r="W17"/>
-      <c s="30" r="X17"/>
-      <c s="30" r="Y17"/>
-      <c s="31" r="Z17"/>
+      <c t="s" s="19" r="D17">
+        <v>103</v>
+      </c>
+      <c t="s" s="18" r="E17">
+        <v>104</v>
+      </c>
+      <c t="s" s="13" r="F17">
+        <v>105</v>
+      </c>
+      <c t="s" s="17" r="G17">
+        <v>106</v>
+      </c>
+      <c t="s" s="11" r="H17">
+        <v>107</v>
+      </c>
+      <c t="s" s="16" r="I17">
+        <v>108</v>
+      </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c t="s" s="15" r="B18">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>105</v>
-      </c>
-      <c t="s" s="11" r="D18">
-        <v>106</v>
-      </c>
-      <c t="s" s="16" r="E18">
-        <v>107</v>
+        <v>111</v>
+      </c>
+      <c t="s" s="19" r="D18">
+        <v>112</v>
+      </c>
+      <c t="s" s="18" r="E18">
+        <v>113</v>
       </c>
       <c t="s" s="13" r="F18">
-        <v>108</v>
-      </c>
-      <c t="s" s="17" r="G18">
-        <v>109</v>
+        <v>114</v>
+      </c>
+      <c t="s" s="20" r="G18">
+        <v>115</v>
       </c>
       <c t="s" s="11" r="H18">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c t="s" s="16" r="I18">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>112</v>
-      </c>
-      <c t="s" s="15" r="B19">
-        <v>113</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>114</v>
-      </c>
-      <c t="s" s="19" r="D19">
-        <v>115</v>
-      </c>
-      <c t="s" s="18" r="E19">
-        <v>116</v>
-      </c>
-      <c t="s" s="13" r="F19">
-        <v>117</v>
-      </c>
-      <c t="s" s="13" r="G19">
+      <c t="s" s="29" r="A19">
         <v>118</v>
       </c>
-      <c t="s" s="11" r="H19">
+      <c s="30" r="B19"/>
+      <c s="30" r="C19"/>
+      <c s="30" r="D19"/>
+      <c s="30" r="E19"/>
+      <c s="30" r="F19"/>
+      <c s="30" r="G19"/>
+      <c s="30" r="H19"/>
+      <c s="30" r="I19"/>
+      <c s="30" r="J19"/>
+      <c s="30" r="K19"/>
+      <c s="30" r="L19"/>
+      <c s="30" r="M19"/>
+      <c s="30" r="N19"/>
+      <c s="30" r="O19"/>
+      <c s="30" r="P19"/>
+      <c s="30" r="Q19"/>
+      <c s="30" r="R19"/>
+      <c s="30" r="S19"/>
+      <c s="30" r="T19"/>
+      <c s="30" r="U19"/>
+      <c s="30" r="V19"/>
+      <c s="30" r="W19"/>
+      <c s="30" r="X19"/>
+      <c s="30" r="Y19"/>
+      <c s="31" r="Z19"/>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
         <v>119</v>
       </c>
-      <c t="s" s="11" r="I19">
+      <c t="s" s="15" r="B20">
         <v>120</v>
       </c>
-    </row>
-    <row r="20">
-      <c s="2" r="A20"/>
-      <c s="2" r="B20"/>
-      <c s="2" r="C20"/>
-      <c s="3" r="D20"/>
-      <c s="3" r="E20"/>
+      <c t="s" s="1" r="C20">
+        <v>121</v>
+      </c>
+      <c t="s" s="11" r="D20">
+        <v>122</v>
+      </c>
+      <c t="s" s="16" r="E20">
+        <v>123</v>
+      </c>
       <c t="s" s="13" r="F20">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c t="s" s="17" r="G20">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c t="s" s="11" r="H20">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c t="s" s="16" r="I20">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
-      <c s="32" r="A21"/>
-      <c s="32" r="B21"/>
-      <c s="32" r="C21"/>
-      <c s="33" r="D21"/>
-      <c s="33" r="E21"/>
-      <c t="s" s="34" r="F21">
-        <v>125</v>
-      </c>
-      <c t="s" s="35" r="G21">
-        <v>126</v>
-      </c>
-      <c t="s" s="36" r="H21">
-        <v>127</v>
-      </c>
-      <c t="s" s="37" r="I21">
+      <c t="s" s="1" r="A21">
         <v>128</v>
       </c>
-      <c s="38" r="J21"/>
-      <c s="38" r="K21"/>
-      <c s="38" r="L21"/>
-      <c s="38" r="M21"/>
-      <c s="38" r="N21"/>
-      <c s="38" r="O21"/>
-      <c s="38" r="P21"/>
-      <c s="38" r="Q21"/>
-      <c s="38" r="R21"/>
-      <c s="38" r="S21"/>
-      <c s="38" r="T21"/>
-      <c s="38" r="U21"/>
-      <c s="38" r="V21"/>
-      <c s="38" r="W21"/>
-      <c s="38" r="X21"/>
-      <c s="38" r="Y21"/>
-      <c s="38" r="Z21"/>
+      <c t="s" s="15" r="B21">
+        <v>129</v>
+      </c>
+      <c t="s" s="1" r="C21">
+        <v>130</v>
+      </c>
+      <c t="s" s="19" r="D21">
+        <v>131</v>
+      </c>
+      <c t="s" s="18" r="E21">
+        <v>132</v>
+      </c>
+      <c t="s" s="13" r="F21">
+        <v>133</v>
+      </c>
+      <c t="s" s="13" r="G21">
+        <v>134</v>
+      </c>
+      <c t="s" s="11" r="H21">
+        <v>135</v>
+      </c>
+      <c t="s" s="11" r="I21">
+        <v>136</v>
+      </c>
     </row>
     <row r="22">
       <c s="2" r="A22"/>
@@ -1546,36 +1593,53 @@
       <c s="3" r="D22"/>
       <c s="3" r="E22"/>
       <c t="s" s="13" r="F22">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c t="s" s="17" r="G22">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c t="s" s="11" r="H22">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c t="s" s="16" r="I22">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23">
-      <c s="2" r="A23"/>
-      <c s="2" r="B23"/>
-      <c s="2" r="C23"/>
-      <c s="3" r="D23"/>
-      <c s="3" r="E23"/>
-      <c t="s" s="13" r="F23">
-        <v>133</v>
-      </c>
-      <c t="s" s="17" r="G23">
-        <v>134</v>
-      </c>
-      <c t="s" s="11" r="H23">
-        <v>135</v>
-      </c>
-      <c t="s" s="16" r="I23">
-        <v>136</v>
-      </c>
+      <c s="32" r="A23"/>
+      <c s="32" r="B23"/>
+      <c s="32" r="C23"/>
+      <c s="33" r="D23"/>
+      <c s="33" r="E23"/>
+      <c t="s" s="34" r="F23">
+        <v>141</v>
+      </c>
+      <c t="s" s="35" r="G23">
+        <v>142</v>
+      </c>
+      <c t="s" s="36" r="H23">
+        <v>143</v>
+      </c>
+      <c t="s" s="37" r="I23">
+        <v>144</v>
+      </c>
+      <c s="38" r="J23"/>
+      <c s="38" r="K23"/>
+      <c s="38" r="L23"/>
+      <c s="38" r="M23"/>
+      <c s="38" r="N23"/>
+      <c s="38" r="O23"/>
+      <c s="38" r="P23"/>
+      <c s="38" r="Q23"/>
+      <c s="38" r="R23"/>
+      <c s="38" r="S23"/>
+      <c s="38" r="T23"/>
+      <c s="38" r="U23"/>
+      <c s="38" r="V23"/>
+      <c s="38" r="W23"/>
+      <c s="38" r="X23"/>
+      <c s="38" r="Y23"/>
+      <c s="38" r="Z23"/>
     </row>
     <row r="24">
       <c s="2" r="A24"/>
@@ -1583,17 +1647,17 @@
       <c s="2" r="C24"/>
       <c s="3" r="D24"/>
       <c s="3" r="E24"/>
-      <c t="s" s="17" r="F24">
-        <v>137</v>
+      <c t="s" s="13" r="F24">
+        <v>145</v>
       </c>
       <c t="s" s="17" r="G24">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c t="s" s="11" r="H24">
-        <v>139</v>
-      </c>
-      <c t="s" s="11" r="I24">
-        <v>140</v>
+        <v>147</v>
+      </c>
+      <c t="s" s="16" r="I24">
+        <v>148</v>
       </c>
     </row>
     <row r="25">
@@ -1603,16 +1667,16 @@
       <c s="3" r="D25"/>
       <c s="3" r="E25"/>
       <c t="s" s="13" r="F25">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c t="s" s="17" r="G25">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c t="s" s="11" r="H25">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c t="s" s="16" r="I25">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26">
@@ -1621,17 +1685,17 @@
       <c s="2" r="C26"/>
       <c s="3" r="D26"/>
       <c s="3" r="E26"/>
-      <c t="s" s="13" r="F26">
-        <v>145</v>
+      <c t="s" s="17" r="F26">
+        <v>153</v>
       </c>
       <c t="s" s="17" r="G26">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c t="s" s="11" r="H26">
-        <v>147</v>
-      </c>
-      <c t="s" s="16" r="I26">
-        <v>148</v>
+        <v>155</v>
+      </c>
+      <c t="s" s="11" r="I26">
+        <v>156</v>
       </c>
     </row>
     <row r="27">
@@ -1641,16 +1705,16 @@
       <c s="3" r="D27"/>
       <c s="3" r="E27"/>
       <c t="s" s="13" r="F27">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c t="s" s="17" r="G27">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c t="s" s="11" r="H27">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c t="s" s="16" r="I27">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28">
@@ -1659,10 +1723,18 @@
       <c s="2" r="C28"/>
       <c s="3" r="D28"/>
       <c s="3" r="E28"/>
-      <c s="4" r="F28"/>
-      <c s="4" r="G28"/>
-      <c s="3" r="H28"/>
-      <c s="3" r="I28"/>
+      <c t="s" s="13" r="F28">
+        <v>161</v>
+      </c>
+      <c t="s" s="17" r="G28">
+        <v>162</v>
+      </c>
+      <c t="s" s="11" r="H28">
+        <v>163</v>
+      </c>
+      <c t="s" s="16" r="I28">
+        <v>164</v>
+      </c>
     </row>
     <row r="29">
       <c s="2" r="A29"/>
@@ -1670,10 +1742,18 @@
       <c s="2" r="C29"/>
       <c s="3" r="D29"/>
       <c s="3" r="E29"/>
-      <c s="4" r="F29"/>
-      <c s="4" r="G29"/>
-      <c s="3" r="H29"/>
-      <c s="3" r="I29"/>
+      <c t="s" s="13" r="F29">
+        <v>165</v>
+      </c>
+      <c t="s" s="17" r="G29">
+        <v>166</v>
+      </c>
+      <c t="s" s="11" r="H29">
+        <v>167</v>
+      </c>
+      <c t="s" s="16" r="I29">
+        <v>168</v>
+      </c>
     </row>
     <row r="30">
       <c s="2" r="A30"/>
@@ -12330,6 +12410,28 @@
       <c s="3" r="D998"/>
       <c s="3" r="E998"/>
       <c s="4" r="F998"/>
+      <c s="4" r="G998"/>
+      <c s="3" r="H998"/>
+      <c s="3" r="I998"/>
+    </row>
+    <row r="999">
+      <c s="2" r="A999"/>
+      <c s="2" r="B999"/>
+      <c s="2" r="C999"/>
+      <c s="3" r="D999"/>
+      <c s="3" r="E999"/>
+      <c s="4" r="F999"/>
+      <c s="4" r="G999"/>
+      <c s="3" r="H999"/>
+      <c s="3" r="I999"/>
+    </row>
+    <row r="1000">
+      <c s="2" r="A1000"/>
+      <c s="2" r="B1000"/>
+      <c s="2" r="C1000"/>
+      <c s="3" r="D1000"/>
+      <c s="3" r="E1000"/>
+      <c s="4" r="F1000"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -12360,43 +12462,49 @@
     <hyperlink ref="E10" r:id="rId25"/>
     <hyperlink ref="G10" r:id="rId26"/>
     <hyperlink ref="I10" r:id="rId27"/>
-    <hyperlink ref="B12" r:id="rId28"/>
-    <hyperlink ref="E12" r:id="rId29"/>
-    <hyperlink ref="G12" r:id="rId30"/>
-    <hyperlink ref="B14" r:id="rId31"/>
-    <hyperlink ref="E14" r:id="rId32"/>
-    <hyperlink ref="G14" r:id="rId33"/>
-    <hyperlink ref="B15" r:id="rId34"/>
-    <hyperlink ref="E15" r:id="rId35"/>
-    <hyperlink ref="G15" r:id="rId36"/>
-    <hyperlink ref="I15" r:id="rId37"/>
-    <hyperlink ref="B16" r:id="rId38"/>
-    <hyperlink ref="E16" r:id="rId39"/>
-    <hyperlink ref="G16" r:id="rId40"/>
-    <hyperlink ref="I16" r:id="rId41"/>
-    <hyperlink ref="B18" r:id="rId42"/>
-    <hyperlink ref="E18" r:id="rId43"/>
-    <hyperlink ref="G18" r:id="rId44"/>
-    <hyperlink ref="I18" r:id="rId45"/>
-    <hyperlink ref="B19" r:id="rId46"/>
-    <hyperlink ref="E19" r:id="rId47"/>
-    <hyperlink ref="G20" r:id="rId48"/>
-    <hyperlink ref="I20" r:id="rId49"/>
-    <hyperlink ref="G21" r:id="rId50"/>
-    <hyperlink ref="I21" r:id="rId51"/>
-    <hyperlink ref="G22" r:id="rId52"/>
-    <hyperlink ref="I22" r:id="rId53"/>
-    <hyperlink ref="G23" r:id="rId54"/>
-    <hyperlink ref="I23" r:id="rId55"/>
-    <hyperlink ref="F24" r:id="rId56"/>
-    <hyperlink ref="G24" r:id="rId57"/>
-    <hyperlink ref="G25" r:id="rId58"/>
-    <hyperlink ref="I25" r:id="rId59"/>
-    <hyperlink ref="G26" r:id="rId60"/>
-    <hyperlink ref="I26" r:id="rId61"/>
-    <hyperlink ref="G27" r:id="rId62"/>
-    <hyperlink ref="I27" r:id="rId63"/>
+    <hyperlink ref="B11" r:id="rId28"/>
+    <hyperlink ref="G11" r:id="rId29"/>
+    <hyperlink ref="I11" r:id="rId30"/>
+    <hyperlink ref="B12" r:id="rId31"/>
+    <hyperlink ref="G12" r:id="rId32"/>
+    <hyperlink ref="I12" r:id="rId33"/>
+    <hyperlink ref="B14" r:id="rId34"/>
+    <hyperlink ref="E14" r:id="rId35"/>
+    <hyperlink ref="G14" r:id="rId36"/>
+    <hyperlink ref="B16" r:id="rId37"/>
+    <hyperlink ref="E16" r:id="rId38"/>
+    <hyperlink ref="G16" r:id="rId39"/>
+    <hyperlink ref="B17" r:id="rId40"/>
+    <hyperlink ref="E17" r:id="rId41"/>
+    <hyperlink ref="G17" r:id="rId42"/>
+    <hyperlink ref="I17" r:id="rId43"/>
+    <hyperlink ref="B18" r:id="rId44"/>
+    <hyperlink ref="E18" r:id="rId45"/>
+    <hyperlink ref="G18" r:id="rId46"/>
+    <hyperlink ref="I18" r:id="rId47"/>
+    <hyperlink ref="B20" r:id="rId48"/>
+    <hyperlink ref="E20" r:id="rId49"/>
+    <hyperlink ref="G20" r:id="rId50"/>
+    <hyperlink ref="I20" r:id="rId51"/>
+    <hyperlink ref="B21" r:id="rId52"/>
+    <hyperlink ref="E21" r:id="rId53"/>
+    <hyperlink ref="G22" r:id="rId54"/>
+    <hyperlink ref="I22" r:id="rId55"/>
+    <hyperlink ref="G23" r:id="rId56"/>
+    <hyperlink ref="I23" r:id="rId57"/>
+    <hyperlink ref="G24" r:id="rId58"/>
+    <hyperlink ref="I24" r:id="rId59"/>
+    <hyperlink ref="G25" r:id="rId60"/>
+    <hyperlink ref="I25" r:id="rId61"/>
+    <hyperlink ref="F26" r:id="rId62"/>
+    <hyperlink ref="G26" r:id="rId63"/>
+    <hyperlink ref="G27" r:id="rId64"/>
+    <hyperlink ref="I27" r:id="rId65"/>
+    <hyperlink ref="G28" r:id="rId66"/>
+    <hyperlink ref="I28" r:id="rId67"/>
+    <hyperlink ref="G29" r:id="rId68"/>
+    <hyperlink ref="I29" r:id="rId69"/>
   </hyperlinks>
-  <drawing r:id="rId64"/>
+  <drawing r:id="rId70"/>
 </worksheet>
 </file>
</xml_diff>